<commit_message>
fif issee user feedback
</commit_message>
<xml_diff>
--- a/public/temp/Jadepay_Onboarded_Customer_Data_Template.xlsx
+++ b/public/temp/Jadepay_Onboarded_Customer_Data_Template.xlsx
@@ -33,8 +33,7 @@
     <t>Passport</t>
   </si>
   <si>
-    <t xml:space="preserve">DOB 
-(MM/DD/YYYY)</t>
+    <t xml:space="preserve">DOB (MM/DD/YYYY)</t>
   </si>
   <si>
     <t xml:space="preserve">Issue Date</t>
@@ -139,7 +138,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -350,11 +348,11 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
+        <bottom style="none"/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -366,11 +364,11 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
+        <bottom style="none"/>
+        <diagonal style="none"/>
       </border>
     </dxf>
   </dxfs>
@@ -915,7 +913,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>

</xml_diff>